<commit_message>
Update formula in cell B23
Update formula in cell B23
</commit_message>
<xml_diff>
--- a/Data Science/Data Science Binomial Distribution.xlsx
+++ b/Data Science/Data Science Binomial Distribution.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenyp\myProjects\The-Tech-Academy-Projects\Data Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED4BDE-55AC-4837-B202-09CD6411BEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F248B3C-1C87-4D52-8970-112F509A9DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5F95BECF-6EFF-4C3D-A8A7-EB6AA1E31D38}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{5F95BECF-6EFF-4C3D-A8A7-EB6AA1E31D38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Step 255" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Step 255'!$A$1:$B$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>ASSIGNMENT</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Factorial of 10 -7</t>
-  </si>
-  <si>
-    <t>There is an approximately .73% chance in binomial distribution that 7 out of 10 kids would prefer dogs over cats.</t>
   </si>
   <si>
     <t>Factorial of (10-7)! Cancels out the frequency factorial in line of kids (10)</t>
@@ -88,9 +85,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -157,7 +155,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -171,7 +169,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -179,6 +177,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -498,41 +497,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.08984375" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -540,7 +537,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -548,7 +545,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -556,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -564,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -572,15 +569,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -589,7 +586,7 @@
         <v>3628800</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -598,7 +595,7 @@
         <v>5040</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -607,19 +604,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="7">
         <f>10*9*8*7*6*5*4</f>
         <v>604800</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -628,7 +625,7 @@
         <v>5040</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>"There are "&amp;B20&amp;" different ways that "&amp;B9&amp;" out of "&amp;B8&amp;" kids could prefer dogs over cats, whether they be the first "&amp;B9&amp; "or scattered in throughout."</f>
         <v>There are 120 different ways that 7 out of 10 kids could prefer dogs over cats, whether they be the first 7or scattered in throughout.</v>
@@ -638,12 +635,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -651,23 +648,26 @@
         <f xml:space="preserve"> (0.5)^7</f>
         <v>7.8125E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="5">
-        <f xml:space="preserve"> (0.5)^7</f>
-        <v>7.8125E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
-        <v>16</v>
+        <f xml:space="preserve"> (0.5)^3</f>
+        <v>0.125</v>
+      </c>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="str">
+        <f>"There is an approximately "&amp;ROUND(B25*100,2)&amp;"% chance in binomial distribution that "&amp;B9&amp;" out of "&amp;B8&amp;" kids would prefer dogs over cats."</f>
+        <v>There is an approximately 11.72% chance in binomial distribution that 7 out of 10 kids would prefer dogs over cats.</v>
       </c>
       <c r="B25" s="10">
         <f>B20*B22*B23</f>
-        <v>7.32421875E-3</v>
+        <v>0.1171875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>